<commit_message>
change text file(from each sheet) name
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/testtest.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/testtest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499F9ED1-B936-FB4C-BF30-8B3FFFA8FD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4363C599-6BD9-9640-AB49-B4BD108BD87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22140" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="MSC" sheetId="5" r:id="rId6"/>
     <sheet name="전공필수" sheetId="6" r:id="rId7"/>
     <sheet name="유사교과목(대체교과목)" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="138">
   <si>
     <t>입력하려는 졸업기준의 학과(전공)명을 선택하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -558,6 +559,22 @@
   </si>
   <si>
     <t>입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>심화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신입학생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -981,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1023,6 +1040,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
@@ -1034,6 +1054,9 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
@@ -1045,6 +1068,9 @@
       <c r="C4" t="s">
         <v>45</v>
       </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
@@ -1056,6 +1082,9 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>2016</v>
+      </c>
       <c r="E5" t="s">
         <v>34</v>
       </c>
@@ -1067,6 +1096,9 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>2016</v>
+      </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
@@ -1109,6 +1141,9 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
+      <c r="D9">
+        <v>21</v>
+      </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
@@ -1151,6 +1186,9 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
@@ -1207,6 +1245,9 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
+      <c r="D16">
+        <v>28</v>
+      </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
@@ -1238,6 +1279,9 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
+      <c r="D18">
+        <v>42</v>
+      </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
@@ -1252,6 +1296,9 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
+      <c r="D19">
+        <v>84</v>
+      </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
@@ -1339,6 +1386,9 @@
       <c r="C25" t="s">
         <v>41</v>
       </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
       <c r="E25" t="s">
         <v>55</v>
       </c>
@@ -1353,6 +1403,9 @@
       <c r="C26" t="s">
         <v>42</v>
       </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
       <c r="E26" t="s">
         <v>55</v>
       </c>
@@ -1367,6 +1420,9 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
       <c r="E27" t="s">
         <v>43</v>
       </c>
@@ -1381,6 +1437,9 @@
       <c r="C28" t="s">
         <v>52</v>
       </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
@@ -1395,6 +1454,9 @@
       <c r="C29" t="s">
         <v>44</v>
       </c>
+      <c r="D29" t="s">
+        <v>137</v>
+      </c>
       <c r="E29" t="s">
         <v>55</v>
       </c>
@@ -1409,6 +1471,9 @@
       <c r="C30" t="s">
         <v>47</v>
       </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
       <c r="E30" t="s">
         <v>55</v>
       </c>
@@ -1423,6 +1488,9 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
+      <c r="D31">
+        <v>140</v>
+      </c>
       <c r="E31" t="s">
         <v>25</v>
       </c>
@@ -1437,6 +1505,9 @@
       <c r="C32" t="s">
         <v>26</v>
       </c>
+      <c r="D32">
+        <v>2.5</v>
+      </c>
       <c r="E32" t="s">
         <v>27</v>
       </c>
@@ -1482,6 +1553,9 @@
       <c r="C35" t="s">
         <v>30</v>
       </c>
+      <c r="D35" t="s">
+        <v>137</v>
+      </c>
       <c r="E35" t="s">
         <v>54</v>
       </c>
@@ -1496,6 +1570,9 @@
       <c r="C36" t="s">
         <v>48</v>
       </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
       <c r="E36" t="s">
         <v>25</v>
       </c>
@@ -1510,6 +1587,9 @@
       <c r="C37" t="s">
         <v>61</v>
       </c>
+      <c r="D37" t="s">
+        <v>92</v>
+      </c>
       <c r="E37" t="s">
         <v>54</v>
       </c>
@@ -1527,6 +1607,9 @@
       <c r="C38" t="s">
         <v>62</v>
       </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
       <c r="E38" t="s">
         <v>25</v>
       </c>
@@ -1540,6 +1623,9 @@
       </c>
       <c r="C39" t="s">
         <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
       </c>
       <c r="E39" t="s">
         <v>54</v>
@@ -1577,7 +1663,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2712,4 +2798,17 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993884BE-283C-BC42-97CF-C46125B7C789}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>